<commit_message>
Actualización scrips, imagenes, tabla descriptiva
</commit_message>
<xml_diff>
--- a/Documentos/Tablas descriptivas.xlsx
+++ b/Documentos/Tablas descriptivas.xlsx
@@ -138,9 +138,6 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -153,13 +150,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,76 +453,76 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="2:6" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="2:6" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
         <v>1624.41</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>2536.0169999999998</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>4153.91</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>1907.06</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>25253400</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>142961979</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>591245300</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>82310700</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>-1.7</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>-9.0629180000000004E-2</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>2.6</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>-0.3</v>
       </c>
     </row>
@@ -540,7 +540,7 @@
   <dimension ref="B3:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,332 +549,432 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10">
-        <v>0</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
         <v>40840.879999999997</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="8">
         <v>410146</v>
       </c>
-      <c r="G4" s="10">
-        <v>0</v>
-      </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="10">
+      <c r="B5" s="10"/>
+      <c r="C5" s="8">
         <v>1</v>
       </c>
-      <c r="D5" s="10">
-        <v>0</v>
-      </c>
-      <c r="E5" s="10">
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
         <v>40902</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>150459</v>
       </c>
-      <c r="G5" s="10">
-        <v>0</v>
-      </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="10">
+      <c r="B6" s="10"/>
+      <c r="C6" s="8">
         <v>2</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>41015</v>
+      </c>
+      <c r="F6" s="8">
+        <v>149262</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="10">
+      <c r="B7" s="10"/>
+      <c r="C7" s="8">
         <v>3</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>41143</v>
+      </c>
+      <c r="F7" s="8">
+        <v>150294</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="10">
+      <c r="B8" s="10"/>
+      <c r="C8" s="8">
         <v>4</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>41051</v>
+      </c>
+      <c r="F8" s="8">
+        <v>147386</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="10">
+      <c r="B9" s="10"/>
+      <c r="C9" s="8">
         <v>5</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="10">
+      <c r="B10" s="10"/>
+      <c r="C10" s="8">
         <v>6</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="10">
+      <c r="B11" s="10"/>
+      <c r="C11" s="8">
         <v>7</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="10">
+      <c r="B12" s="10"/>
+      <c r="C12" s="8">
         <v>8</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="10">
+      <c r="B13" s="10"/>
+      <c r="C13" s="8">
         <v>9</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="10">
+      <c r="B14" s="10"/>
+      <c r="C14" s="8">
         <v>10</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="10">
+      <c r="B15" s="10"/>
+      <c r="C15" s="8">
         <v>11</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
-      <c r="C16" s="10">
+      <c r="B16" s="10"/>
+      <c r="C16" s="8">
         <v>12</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="C17" s="10">
+      <c r="B17" s="10"/>
+      <c r="C17" s="8">
         <v>13</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="10">
+      <c r="B18" s="10"/>
+      <c r="C18" s="8">
         <v>14</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="10">
+      <c r="B19" s="10"/>
+      <c r="C19" s="8">
         <v>15</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="10">
+      <c r="B20" s="10"/>
+      <c r="C20" s="8">
         <v>16</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
-      <c r="C21" s="10">
+      <c r="B21" s="10"/>
+      <c r="C21" s="8">
         <v>17</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
-      <c r="C22" s="10">
+      <c r="B22" s="10"/>
+      <c r="C22" s="8">
         <v>18</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="8"/>
-      <c r="C23" s="10">
+      <c r="B23" s="10"/>
+      <c r="C23" s="8">
         <v>19</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8">
+        <v>0</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="8"/>
-      <c r="C24" s="10">
+      <c r="B24" s="10"/>
+      <c r="C24" s="8">
         <v>20</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
-      <c r="C25" s="10">
+      <c r="B25" s="10"/>
+      <c r="C25" s="8">
         <v>21</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="D25" s="8">
+        <v>0</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8">
+        <v>0</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="8"/>
-      <c r="C26" s="10">
+      <c r="B26" s="10"/>
+      <c r="C26" s="8">
         <v>22</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8">
+        <v>0</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-      <c r="C27" s="10">
+      <c r="B27" s="10"/>
+      <c r="C27" s="8">
         <v>23</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
+      <c r="D27" s="8">
+        <v>0</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8">
+        <v>0</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>